<commit_message>
chore(data): update GreatLink data
</commit_message>
<xml_diff>
--- a/data/GreatLink/GreatLink Asia Dividend Advantage_Dividends.xlsx
+++ b/data/GreatLink/GreatLink Asia Dividend Advantage_Dividends.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DividendHistory" sheetId="1" r:id="GemRid825248"/>
+    <sheet name="DividendHistory" sheetId="1" r:id="GemRid510399"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>XD Date</t>
   </si>
@@ -26,10 +26,13 @@
     <t>Gross Dividend</t>
   </si>
   <si>
+    <t>06/01/2025</t>
+  </si>
+  <si>
+    <t>0.010</t>
+  </si>
+  <si>
     <t>03/10/2024</t>
-  </si>
-  <si>
-    <t>0.010</t>
   </si>
   <si>
     <t>03/07/2024</t>
@@ -394,6 +397,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="1.8" right="1.8" top="1.8999999999999999" bottom="1.8999999999999999" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" scale="100" paperSize="0" firstPageNumber="1" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>

</xml_diff>

<commit_message>
chore(data): update data except MSCI
</commit_message>
<xml_diff>
--- a/data/GreatLink/GreatLink Asia Dividend Advantage_Dividends.xlsx
+++ b/data/GreatLink/GreatLink Asia Dividend Advantage_Dividends.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DividendHistory" sheetId="1" r:id="GemRid653477"/>
+    <sheet name="DividendHistory" sheetId="1" r:id="GemRid39615"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>XD Date</t>
   </si>
@@ -26,10 +26,13 @@
     <t>Gross Dividend</t>
   </si>
   <si>
+    <t>03/10/2025</t>
+  </si>
+  <si>
+    <t>0.010</t>
+  </si>
+  <si>
     <t>03/07/2025</t>
-  </si>
-  <si>
-    <t>0.010</t>
   </si>
   <si>
     <t>03/04/2025</t>
@@ -436,6 +439,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="1.8" right="1.8" top="1.8999999999999999" bottom="1.8999999999999999" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" scale="100" paperSize="0" firstPageNumber="1" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>

</xml_diff>